<commit_message>
Update part 2 of 3 rubric, add submission writeup
</commit_message>
<xml_diff>
--- a/admin/ProjectRubric2of3.xlsx
+++ b/admin/ProjectRubric2of3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elari\Documents\Repos\CSCI_S71\Teamify\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC6BE20-9039-4210-955B-460198BBA42F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1D309E-FDFD-4826-A046-8C8F84E06B21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16665" yWindow="-15045" windowWidth="15300" windowHeight="12150" xr2:uid="{240F924D-48B8-43CB-A5F6-3B6DFA99720D}"/>
+    <workbookView xWindow="16635" yWindow="-15930" windowWidth="19125" windowHeight="15930" xr2:uid="{240F924D-48B8-43CB-A5F6-3B6DFA99720D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>2.0 pts</t>
   </si>
@@ -143,13 +143,34 @@
     <t>Specification completed as written.  Tasks are labeled and linked to PBI's in Trello.</t>
   </si>
   <si>
-    <t>The Trello board includes both PBI's and tasks, which are linked.  The progress of all work items is represented by the list (column) they are in.  Need to update the README</t>
-  </si>
-  <si>
-    <t>An initial burndown chart is created.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We forecast 10pts. Based on the scale that was used in our estimation activity.  Sprint Goal:  Display resgistered students and team names.    Need to update the README </t>
+    <t xml:space="preserve">We forecast 10pts. Based on the scale that was used in our estimation activity.  Sprint Goal:  Display resgistered students and team names.    </t>
+  </si>
+  <si>
+    <t>The Trello board includes both PBI's and tasks, which are linked.  The progress of all work items is represented by the list (column) they are in.  An explanation of the board layout was provided in the README.</t>
+  </si>
+  <si>
+    <t>A burndown chart was created as stated with expected, planned and actual lines.  It was updated daily.</t>
+  </si>
+  <si>
+    <t>A daily scrum has been conducted every day since 6/28/20 and documented in a log with three sections as specified.</t>
+  </si>
+  <si>
+    <t>The burndown chart is in the repo.  URLs for the burndown and the task board are in the README</t>
+  </si>
+  <si>
+    <t>We mob programmed for the entire Sprint. Several photos are in the repo.  Links and photos are in the README.</t>
+  </si>
+  <si>
+    <t>We used TDD for the entire sprint.  We have atotal of 21 tests written with 52 assertions that all pass.  Anu confirmed the evidence in our README met requirements.</t>
+  </si>
+  <si>
+    <t>Scheduled for 7/6/20, 1PM</t>
+  </si>
+  <si>
+    <t>Our app was pushed to the production server and works well.</t>
+  </si>
+  <si>
+    <t>Richard is scheduled to meet with us at our Sprint Review on'7/6/20, 1PM</t>
   </si>
 </sst>
 </file>
@@ -580,7 +601,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -624,10 +645,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="E4" s="3">
+        <v>44016</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -638,7 +662,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="E5" s="3">
+        <v>44016</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>34</v>
@@ -703,10 +730,13 @@
         <v>2</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="E9" s="3">
+        <v>44016</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -717,10 +747,13 @@
         <v>14</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="E10" s="3">
+        <v>44017</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -731,7 +764,13 @@
         <v>4</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="E11" s="3">
+        <v>44017</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -742,7 +781,13 @@
         <v>4</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="E12" s="3">
+        <v>44017</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -753,7 +798,13 @@
         <v>4</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="E13" s="3">
+        <v>44017</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -764,7 +815,13 @@
         <v>2</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="E14" s="3">
+        <v>44017</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -775,7 +832,13 @@
         <v>0</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="E15" s="3">
+        <v>44016</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -786,10 +849,16 @@
         <v>4</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+      <c r="E16" s="3">
+        <v>44017</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -797,10 +866,16 @@
         <v>3</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+      <c r="E17" s="3">
+        <v>44017</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
@@ -810,8 +885,11 @@
       <c r="D18" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="2" t="s">
         <v>29</v>
       </c>
@@ -819,10 +897,16 @@
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="62.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+      <c r="E19" s="3">
+        <v>44017</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="62.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
@@ -831,6 +915,9 @@
       </c>
       <c r="D20" s="7" t="s">
         <v>11</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated part 2 of 3 rubric tracker
</commit_message>
<xml_diff>
--- a/admin/ProjectRubric2of3.xlsx
+++ b/admin/ProjectRubric2of3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elari\Documents\Repos\CSCI_S71\Teamify\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1D309E-FDFD-4826-A046-8C8F84E06B21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE776E8B-C231-421A-A62E-1F1C473DCDE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16635" yWindow="-15930" windowWidth="19125" windowHeight="15930" xr2:uid="{240F924D-48B8-43CB-A5F6-3B6DFA99720D}"/>
+    <workbookView xWindow="17565" yWindow="-14325" windowWidth="19125" windowHeight="12810" xr2:uid="{240F924D-48B8-43CB-A5F6-3B6DFA99720D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>2.0 pts</t>
   </si>
@@ -68,9 +68,6 @@
     <t xml:space="preserve">Date </t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Rubric Tracking for Assignment 2:  First Sprint</t>
   </si>
   <si>
@@ -164,13 +161,13 @@
     <t>We used TDD for the entire sprint.  We have atotal of 21 tests written with 52 assertions that all pass.  Anu confirmed the evidence in our README met requirements.</t>
   </si>
   <si>
-    <t>Scheduled for 7/6/20, 1PM</t>
-  </si>
-  <si>
     <t>Our app was pushed to the production server and works well.</t>
   </si>
   <si>
-    <t>Richard is scheduled to meet with us at our Sprint Review on'7/6/20, 1PM</t>
+    <t>Scheduled for 7/6/20, 1PM - Completed</t>
+  </si>
+  <si>
+    <t>Richard and Anu met with us at our Sprint Review on 7/6/20, 1PM.  We received valuable feedback on product features that confirmed our backlog.</t>
   </si>
 </sst>
 </file>
@@ -601,7 +598,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -617,7 +614,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -639,251 +636,254 @@
     </row>
     <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="3">
         <v>44016</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="3">
         <v>44016</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="3">
         <v>44014</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="78.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="3">
         <v>44013</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3">
         <v>44014</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3">
         <v>44016</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3">
         <v>44017</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="3">
         <v>44017</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="3">
         <v>44017</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="3">
         <v>44017</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="3">
         <v>44017</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3">
         <v>44016</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="3">
         <v>44017</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3">
         <v>44017</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="E18" s="3">
+        <v>44018</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>43</v>
@@ -891,33 +891,36 @@
     </row>
     <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="3">
         <v>44017</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="62.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="E20" s="3">
+        <v>44018</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>